<commit_message>
Added Some for youtube channels
</commit_message>
<xml_diff>
--- a/Learning YouTube Channels/YouTube Channels.xlsx
+++ b/Learning YouTube Channels/YouTube Channels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Personal-GIT\Learning\YouTube Channels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Personal-GIT\Learning\Learning YouTube Channels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D110B6E8-F9C0-47AC-91E7-3D9FF5CBE49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9D1469-3E32-474B-B300-36A66CD78213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="600" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sorted" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="109">
   <si>
     <t>C</t>
   </si>
@@ -221,6 +221,138 @@
   </si>
   <si>
     <t>mycodeschool</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>CloudGuru</t>
+  </si>
+  <si>
+    <t>Fireship</t>
+  </si>
+  <si>
+    <t>AI/ML</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>Algorithms</t>
+  </si>
+  <si>
+    <t>StatQuest</t>
+  </si>
+  <si>
+    <t>LeetCode</t>
+  </si>
+  <si>
+    <t>NeetCode</t>
+  </si>
+  <si>
+    <t>Azure/AWS</t>
+  </si>
+  <si>
+    <t>Blockchain</t>
+  </si>
+  <si>
+    <t>Web Development</t>
+  </si>
+  <si>
+    <t>Net Ninjs</t>
+  </si>
+  <si>
+    <t>Corey Sohafer</t>
+  </si>
+  <si>
+    <t>Cyber Security</t>
+  </si>
+  <si>
+    <t>David Bombal</t>
+  </si>
+  <si>
+    <t>Quick Videos</t>
+  </si>
+  <si>
+    <t>Andrei Karpathy</t>
+  </si>
+  <si>
+    <t>Bro Code</t>
+  </si>
+  <si>
+    <t>Kevin Powell</t>
+  </si>
+  <si>
+    <t>Abdul Bari</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>Andrew Brown</t>
+  </si>
+  <si>
+    <t>Luke Barousse</t>
+  </si>
+  <si>
+    <t>Kunal Kushwaha</t>
+  </si>
+  <si>
+    <t>Krish Naik</t>
+  </si>
+  <si>
+    <t>AR/VR</t>
+  </si>
+  <si>
+    <t>FuseDVR</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>Khan Academy</t>
+  </si>
+  <si>
+    <t>UI/UX</t>
+  </si>
+  <si>
+    <t>GFXMentor</t>
+  </si>
+  <si>
+    <t>Devops</t>
+  </si>
+  <si>
+    <t>Tech world with Nana</t>
+  </si>
+  <si>
+    <t>The Cyber Mentor</t>
+  </si>
+  <si>
+    <t>The Ruby Way</t>
+  </si>
+  <si>
+    <t>Scala</t>
+  </si>
+  <si>
+    <t>Scala Love</t>
+  </si>
+  <si>
+    <t>Kotlin Programming</t>
+  </si>
+  <si>
+    <t>Flutter</t>
+  </si>
+  <si>
+    <t>The Net Ninja</t>
+  </si>
+  <si>
+    <t>FreeCodeCamp.org</t>
+  </si>
+  <si>
+    <t>The Cherno</t>
+  </si>
+  <si>
+    <t>Programming With Mosh</t>
   </si>
 </sst>
 </file>
@@ -548,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,6 +906,262 @@
       </c>
       <c r="B27" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -789,7 +1177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4910AEB1-F023-407D-B4CA-B032422A6373}">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>